<commit_message>
Added sure-fire plugin in pom.xml ....
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\Batch12thOct2019WebDriver\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DDT_Framework_Concept\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D98A48-0F5B-4F1F-A921-FB4FCD72ED80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31322164-4D6B-4A73-92F1-D3348C2C213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{715FCD43-313D-4EF8-8A46-98E7F8392753}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{715FCD43-313D-4EF8-8A46-98E7F8392753}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginTest" sheetId="2" r:id="rId1"/>
+    <sheet name="ValidateLogin" sheetId="2" r:id="rId1"/>
     <sheet name="addCustomer" sheetId="3" r:id="rId2"/>
     <sheet name="openAccount" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395160BC-4615-4C74-8658-60B81C5A4647}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B48979-AD56-4433-A793-B51ECEB257DA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>